<commit_message>
Update InterFace imposible for VanLang Logo
</commit_message>
<xml_diff>
--- a/Sep2018_MVC/Files/attendance.xlsx
+++ b/Sep2018_MVC/Files/attendance.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DF53DD2C-BF89-4CFF-8086-754FB3518BAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{081ADD08-5CDC-4627-ADC1-E92A0F263D36}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,8 +568,8 @@
         <v>22</v>
       </c>
       <c r="C7" s="3">
-        <f>DATE(2018,7,19)</f>
-        <v>43300</v>
+        <f>DATE(2018,7,21)</f>
+        <v>43302</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>30</v>
@@ -598,10 +598,10 @@
         <v>35</v>
       </c>
       <c r="F8" s="4">
-        <v>0.375</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="G8" s="5">
-        <v>0.5</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="H8" s="1">
         <v>3</v>

</xml_diff>